<commit_message>
updates to the joss paper
</commit_message>
<xml_diff>
--- a/paper/benchmarking/GCMC isotherms/GCMC_calculated_areas_and_software_settings.xlsx
+++ b/paper/benchmarking/GCMC isotherms/GCMC_calculated_areas_and_software_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gianmarcoterrones/Research/MOFs/Greg_SESAMI/SESAMI_web/paper/benchmarking/GCMC isotherms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4059E4-38D9-604E-A7D5-715672A87D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D6406A-B327-1F46-9D74-1DAB01890664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32160" yWindow="11640" windowWidth="28800" windowHeight="16320" activeTab="1" xr2:uid="{E941D5A1-A0F3-0B48-A4F6-A2D24C9292E4}"/>
+    <workbookView xWindow="32160" yWindow="11640" windowWidth="28800" windowHeight="16320" xr2:uid="{E941D5A1-A0F3-0B48-A4F6-A2D24C9292E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -276,13 +276,13 @@
     <t>So, probe radius of 2.27A, and 2000 MC samples per atom</t>
   </si>
   <si>
-    <t>Note: SIFSIX was not analyzed due to its poor GCMC isotherm</t>
-  </si>
-  <si>
     <t>SESAMI web</t>
   </si>
   <si>
     <t>Using the default options for BETSI (BETSI option set 1)</t>
+  </si>
+  <si>
+    <t>Note: SIFSIX-3 (Ni) was not analyzed due to its poor GCMC isotherm</t>
   </si>
 </sst>
 </file>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC01AB12-853D-2D46-8C97-B39D3FCBFBBF}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1387,7 +1387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685C9287-4B61-3F4F-A0D7-84642B1E885B}">
   <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -1403,7 +1403,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1453,7 +1453,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
changes to joss supplementary files
</commit_message>
<xml_diff>
--- a/paper/benchmarking/GCMC isotherms/GCMC_calculated_areas_and_software_settings.xlsx
+++ b/paper/benchmarking/GCMC isotherms/GCMC_calculated_areas_and_software_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gianmarcoterrones/Research/MOFs/Greg_SESAMI/SESAMI_web/paper/benchmarking/GCMC isotherms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D6406A-B327-1F46-9D74-1DAB01890664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA791DF3-04FC-7642-AAF9-3A47F40D7DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32160" yWindow="11640" windowWidth="28800" windowHeight="16320" xr2:uid="{E941D5A1-A0F3-0B48-A4F6-A2D24C9292E4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" activeTab="1" xr2:uid="{E941D5A1-A0F3-0B48-A4F6-A2D24C9292E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="84">
   <si>
     <t>Using the default options on https://sesami-web.org/</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>Note: SIFSIX-3 (Ni) was not analyzed due to its poor GCMC isotherm</t>
+  </si>
+  <si>
+    <t>Custom adsorbate</t>
   </si>
 </sst>
 </file>
@@ -731,7 +734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC01AB12-853D-2D46-8C97-B39D3FCBFBBF}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -1385,10 +1388,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685C9287-4B61-3F4F-A0D7-84642B1E885B}">
-  <dimension ref="A1:C106"/>
+  <dimension ref="A1:C107"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1416,73 +1419,73 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>0.99950000000000006</v>
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0.99950000000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>0.998</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16">
-        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17">
-        <v>0.995</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>0.995</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
@@ -1490,7 +1493,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
         <v>28</v>
@@ -1498,7 +1501,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
         <v>28</v>
@@ -1506,54 +1509,54 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>32</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="13" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30">
-        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31">
-        <v>0.995</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="B32">
+        <v>0.995</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B33" t="s">
         <v>28</v>
@@ -1561,15 +1564,15 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B35" t="s">
         <v>8</v>
@@ -1577,36 +1580,36 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="8" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="8" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42">
-        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B43">
-        <v>0.998</v>
+        <v>10</v>
       </c>
       <c r="C43" t="s">
         <v>46</v>
@@ -1614,15 +1617,15 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>27</v>
-      </c>
-      <c r="B44" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="B44">
+        <v>0.998</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B45" t="s">
         <v>28</v>
@@ -1630,15 +1633,15 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B47" t="s">
         <v>8</v>
@@ -1646,66 +1649,66 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B48" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="8" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="8" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="8" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="8" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>47</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>49</v>
-      </c>
-      <c r="B63" t="s">
-        <v>28</v>
+        <v>47</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B64" t="s">
         <v>28</v>
@@ -1713,15 +1716,15 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B65" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B66" t="s">
         <v>8</v>
@@ -1729,51 +1732,51 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>52</v>
+      </c>
+      <c r="B67" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>53</v>
       </c>
-      <c r="B67">
+      <c r="B68">
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="8" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="8" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="8" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>47</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>49</v>
-      </c>
-      <c r="B76" t="s">
-        <v>28</v>
+        <v>47</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B77" t="s">
         <v>28</v>
@@ -1781,15 +1784,15 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B78" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B79" t="s">
         <v>8</v>
@@ -1797,94 +1800,102 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>52</v>
+      </c>
+      <c r="B80" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>53</v>
       </c>
-      <c r="B80">
+      <c r="B81">
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="8" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" s="8" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A94" s="8" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="8" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100" s="1" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A102" s="8" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="8" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Extension to software comparison and explanation for when software do not find surface areas
</commit_message>
<xml_diff>
--- a/paper/benchmarking/GCMC isotherms/GCMC_calculated_areas_and_software_settings.xlsx
+++ b/paper/benchmarking/GCMC isotherms/GCMC_calculated_areas_and_software_settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gianmarcoterrones/Research/MOFs/Greg_SESAMI/SESAMI_web/paper/benchmarking/GCMC isotherms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA791DF3-04FC-7642-AAF9-3A47F40D7DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9418B3BB-3975-0A48-97BF-29512952038C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" activeTab="1" xr2:uid="{E941D5A1-A0F3-0B48-A4F6-A2D24C9292E4}"/>
   </bookViews>
@@ -1390,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685C9287-4B61-3F4F-A0D7-84642B1E885B}">
   <dimension ref="A1:C107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1611,9 +1611,6 @@
       <c r="B43">
         <v>10</v>
       </c>
-      <c r="C43" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
@@ -1621,6 +1618,9 @@
       </c>
       <c r="B44">
         <v>0.998</v>
+      </c>
+      <c r="C44" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>